<commit_message>
Fixing bug when reading compound shard keys.
</commit_message>
<xml_diff>
--- a/ddl_tools/test_excel_reader.xlsx
+++ b/ddl_tools/test_excel_reader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="45">
   <si>
     <t>Database</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>FK_table3_to_table4</t>
+  </si>
+  <si>
+    <t>column_1,column_2</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -828,13 +831,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -924,6 +928,12 @@
       </c>
       <c r="H3" t="s">
         <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3">
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -983,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>